<commit_message>
Update Fahr_Haltezeiten MGT Gasturbinen_202007082.xlsx
</commit_message>
<xml_diff>
--- a/Fahr_Haltezeiten MGT Gasturbinen_202007082.xlsx
+++ b/Fahr_Haltezeiten MGT Gasturbinen_202007082.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - MDS Aero Support\543 MAN\543 Test Procedure - Automation - Mission Mode\MAN-GTP5-Automation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mdsaero-my.sharepoint.com/personal/joachim_agou_mdsaero_com/Documents/543 MAN/543 Test Procedure - Automation - Mission Mode/MAN-GTP5-Automation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="11_B1396941C32ABDE16E2A1B52076C7673E29E43DE" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6115FDCE-A3C9-431D-AC34-FDEDBBE9EC44}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="11_B1396941C32ABDE16E2A1B52076C7673E29E43DE" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{95CE6C81-6AC6-45D6-B18A-52998385DFC3}"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="-110" windowWidth="37690" windowHeight="21820" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19320" yWindow="0" windowWidth="18630" windowHeight="21330" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tab MGT6000-2S" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="87">
   <si>
     <t>rpm</t>
   </si>
@@ -413,6 +413,12 @@
   </si>
   <si>
     <t>excitation AVR (voltage)</t>
+  </si>
+  <si>
+    <t>kw</t>
+  </si>
+  <si>
+    <t>+-0.1%</t>
   </si>
 </sst>
 </file>
@@ -635,7 +641,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -711,10 +717,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4663,7 +4670,7 @@
         <f t="shared" si="0"/>
         <v>154</v>
       </c>
-      <c r="G33" s="31" t="s">
+      <c r="G33" s="32" t="s">
         <v>40</v>
       </c>
     </row>
@@ -4687,7 +4694,7 @@
         <f t="shared" si="0"/>
         <v>169</v>
       </c>
-      <c r="G34" s="31"/>
+      <c r="G34" s="32"/>
     </row>
     <row r="35" spans="1:7" ht="35.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
@@ -4709,7 +4716,7 @@
         <f t="shared" si="0"/>
         <v>184</v>
       </c>
-      <c r="G35" s="31"/>
+      <c r="G35" s="32"/>
     </row>
     <row r="36" spans="1:7" ht="15.5" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
@@ -5362,10 +5369,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A3:F44"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -5375,6 +5382,14 @@
     <col min="4" max="4" width="14.26953125" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C1">
+        <v>13030</v>
+      </c>
+      <c r="D1">
+        <v>0</v>
+      </c>
+    </row>
     <row r="3" spans="1:6" ht="20" x14ac:dyDescent="0.4">
       <c r="C3" s="15" t="s">
         <v>53</v>
@@ -5393,7 +5408,7 @@
     <row r="7" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:6" s="2" customFormat="1" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" s="2" customFormat="1" ht="25" x14ac:dyDescent="0.25">
       <c r="B8" s="29" t="s">
         <v>67</v>
       </c>
@@ -5771,7 +5786,7 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="32">
+      <c r="B38" s="31">
         <v>0</v>
       </c>
       <c r="C38" s="3"/>
@@ -5798,11 +5813,35 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
+      <c r="D43" s="3">
+        <v>60</v>
+      </c>
+      <c r="E43" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
+      <c r="B44">
+        <v>100</v>
+      </c>
+      <c r="C44" s="3">
+        <v>6000</v>
+      </c>
+      <c r="D44" s="3">
+        <f>0.1*C44</f>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <v>30</v>
+      </c>
+      <c r="C45">
+        <v>1800</v>
+      </c>
+      <c r="E45" s="33" t="s">
+        <v>86</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -5820,7 +5859,7 @@
   </sheetPr>
   <dimension ref="R1:U33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>

</xml_diff>